<commit_message>
Added Test Scenarios for CheckOut
</commit_message>
<xml_diff>
--- a/src/test/resources/TestScenarios.xlsx
+++ b/src/test/resources/TestScenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>SwipeInController</t>
   </si>
@@ -61,6 +61,16 @@
   </si>
   <si>
     <t>StationID is correct according to system</t>
+  </si>
+  <si>
+    <t>SwipeOutController</t>
+  </si>
+  <si>
+    <t>User allowed to get out:
+When Balance meets minimum account balance criteria</t>
+  </si>
+  <si>
+    <t>Actual Fare deducted on the basis of days and Number of Stations</t>
   </si>
 </sst>
 </file>
@@ -123,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -131,6 +141,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -577,9 +591,155 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="22.5" x14ac:dyDescent="0.15">
+      <c r="A22" s="4">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Test Case Added (Given When Then)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestScenarios.xlsx
+++ b/src/test/resources/TestScenarios.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18315" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="18315" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SwipeIn" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>SwipeInController</t>
   </si>
   <si>
     <t>TC No.</t>
-  </si>
-  <si>
-    <t>TestCase</t>
   </si>
   <si>
     <t>Expected</t>
@@ -71,6 +68,54 @@
   </si>
   <si>
     <t>Actual Fare deducted on the basis of days and Number of Stations</t>
+  </si>
+  <si>
+    <t>TestScenarios</t>
+  </si>
+  <si>
+    <t>TestCase No</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Then</t>
+  </si>
+  <si>
+    <t>MetroCard is SwippedIn</t>
+  </si>
+  <si>
+    <t>User Able to CheckIn without Exception</t>
+  </si>
+  <si>
+    <t>User not Able to CheckIn and Exception is thrown "Out of Balance"</t>
+  </si>
+  <si>
+    <t>When CardId has allowed characters 
+And Balance is 5.5
+And StationId is A1
+And Day is Monday</t>
+  </si>
+  <si>
+    <t>When CardId has allowed characters 
+And Balance is 5.4
+And StationId is A1
+And Day is Monday</t>
+  </si>
+  <si>
+    <t>When CardId has allowed characters 
+And Balance is 5.6
+And StationId is A1
+And Day is Monday</t>
+  </si>
+  <si>
+    <t>When CardId has allowed characters  
+And Balance is 5.6
+And StationId is A1
+And Day is Monday</t>
   </si>
 </sst>
 </file>
@@ -92,7 +137,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,19 +184,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -460,28 +515,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -492,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -505,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -518,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -531,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -544,7 +599,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -557,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -570,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -583,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -592,28 +647,28 @@
       <c r="G10" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -624,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -637,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -650,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -663,7 +718,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -676,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -689,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -702,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -715,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -724,11 +779,11 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="22.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>9</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>15</v>
+      <c r="B22" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -748,13 +803,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.625" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>